<commit_message>
Added split models performance metrics.
</commit_message>
<xml_diff>
--- a/data/rungholt/Rungholt.xlsx
+++ b/data/rungholt/Rungholt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maacr\Programming\DEI\src\data\rungholt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9F3891-35EB-4E25-88B8-8349460D756E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9DC56D-9A4C-4313-9BDD-94C7F4135562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="90" windowWidth="28620" windowHeight="15420" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="14265" windowHeight="15420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vert" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>local size</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>meshlets</t>
+  </si>
+  <si>
+    <t>1 passo</t>
+  </si>
+  <si>
+    <t>84 passos</t>
   </si>
 </sst>
 </file>
@@ -9761,15 +9767,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I127"/>
+  <dimension ref="A1:J128"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -9792,8 +9798,11 @@
         <f t="shared" ref="G1:G32" si="0">(1+F1)/(E1-D1)*1000</f>
         <v>215.07226428079835</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>32</v>
       </c>
@@ -9812,7 +9821,7 @@
       <c r="F2">
         <v>2499</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="3">
         <f t="shared" si="0"/>
         <v>147.96401515151513</v>
       </c>
@@ -9823,7 +9832,7 @@
         <v>363501</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>32</v>
       </c>
@@ -9842,7 +9851,7 @@
       <c r="F3">
         <v>2499</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="3">
         <f t="shared" si="0"/>
         <v>147.51003068208638</v>
       </c>
@@ -9853,7 +9862,7 @@
         <v>363501</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>32</v>
       </c>
@@ -9872,7 +9881,7 @@
       <c r="F4">
         <v>2499</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="3">
         <f t="shared" si="0"/>
         <v>145.63672375626237</v>
       </c>
@@ -9883,7 +9892,7 @@
         <v>181777</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>32</v>
       </c>
@@ -9902,7 +9911,7 @@
       <c r="F5">
         <v>2499</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="3">
         <f t="shared" si="0"/>
         <v>145.602795573675</v>
       </c>
@@ -9913,7 +9922,7 @@
         <v>363501</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>32</v>
       </c>
@@ -9932,12 +9941,12 @@
       <c r="F6">
         <v>2499</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="3">
         <f t="shared" si="0"/>
         <v>145.09576320371445</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>32</v>
       </c>
@@ -9956,7 +9965,7 @@
       <c r="F7">
         <v>2499</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>144.83517756792767</v>
       </c>
@@ -9967,616 +9976,619 @@
         <v>181777</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="B8">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>256</v>
+        <v>0</v>
       </c>
       <c r="D8">
+        <v>1067918</v>
+      </c>
+      <c r="E8">
+        <v>1085189</v>
+      </c>
+      <c r="F8">
+        <v>2499</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
+        <v>144.75131723698686</v>
+      </c>
+      <c r="J8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>32</v>
+      </c>
+      <c r="B9">
+        <v>32</v>
+      </c>
+      <c r="C9">
+        <v>256</v>
+      </c>
+      <c r="D9">
         <v>35290</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <v>52575</v>
       </c>
-      <c r="F8">
-        <v>2499</v>
-      </c>
-      <c r="G8" s="2">
+      <c r="F9">
+        <v>2499</v>
+      </c>
+      <c r="G9" s="2">
         <f t="shared" si="0"/>
         <v>144.6340757882557</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>32</v>
-      </c>
-      <c r="B9">
-        <v>64</v>
-      </c>
-      <c r="C9">
-        <v>16</v>
-      </c>
-      <c r="D9">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>32</v>
+      </c>
+      <c r="B10">
+        <v>64</v>
+      </c>
+      <c r="C10">
+        <v>16</v>
+      </c>
+      <c r="D10">
         <v>38362</v>
       </c>
-      <c r="E9">
+      <c r="E10">
         <v>55651</v>
       </c>
-      <c r="F9">
-        <v>2499</v>
-      </c>
-      <c r="G9" s="2">
+      <c r="F10">
+        <v>2499</v>
+      </c>
+      <c r="G10" s="2">
         <f t="shared" si="0"/>
         <v>144.60061310659958</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>32</v>
-      </c>
-      <c r="B10">
-        <v>32</v>
-      </c>
-      <c r="C10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>32</v>
+      </c>
+      <c r="B11">
+        <v>32</v>
+      </c>
+      <c r="C11">
         <v>512</v>
       </c>
-      <c r="D10">
+      <c r="D11">
         <v>35683</v>
       </c>
-      <c r="E10">
+      <c r="E11">
         <v>53130</v>
       </c>
-      <c r="F10">
-        <v>2499</v>
-      </c>
-      <c r="G10" s="2">
+      <c r="F11">
+        <v>2499</v>
+      </c>
+      <c r="G11" s="2">
         <f t="shared" si="0"/>
         <v>143.29111021952198</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>32</v>
-      </c>
-      <c r="B11">
-        <v>64</v>
-      </c>
-      <c r="C11">
-        <v>32</v>
-      </c>
-      <c r="D11">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>32</v>
+      </c>
+      <c r="B12">
+        <v>64</v>
+      </c>
+      <c r="C12">
+        <v>32</v>
+      </c>
+      <c r="D12">
         <v>39182</v>
       </c>
-      <c r="E11">
+      <c r="E12">
         <v>56813</v>
       </c>
-      <c r="F11">
-        <v>2499</v>
-      </c>
-      <c r="G11" s="2">
+      <c r="F12">
+        <v>2499</v>
+      </c>
+      <c r="G12" s="2">
         <f t="shared" si="0"/>
         <v>141.79570075435313</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>32</v>
-      </c>
-      <c r="B12">
-        <v>64</v>
-      </c>
-      <c r="C12">
-        <v>8</v>
-      </c>
-      <c r="D12">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>32</v>
+      </c>
+      <c r="B13">
+        <v>64</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13">
         <v>38356</v>
       </c>
-      <c r="E12">
+      <c r="E13">
         <v>56184</v>
       </c>
-      <c r="F12">
-        <v>2499</v>
-      </c>
-      <c r="G12" s="2">
+      <c r="F13">
+        <v>2499</v>
+      </c>
+      <c r="G13" s="2">
         <f t="shared" si="0"/>
         <v>140.22885348889389</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>32</v>
-      </c>
-      <c r="B13">
-        <v>64</v>
-      </c>
-      <c r="C13">
-        <v>64</v>
-      </c>
-      <c r="D13">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>32</v>
+      </c>
+      <c r="B14">
+        <v>64</v>
+      </c>
+      <c r="C14">
+        <v>64</v>
+      </c>
+      <c r="D14">
         <v>39387</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <v>57251</v>
       </c>
-      <c r="F13">
-        <v>2499</v>
-      </c>
-      <c r="G13" s="2">
+      <c r="F14">
+        <v>2499</v>
+      </c>
+      <c r="G14" s="2">
         <f t="shared" si="0"/>
         <v>139.94626063591582</v>
       </c>
-      <c r="H13">
+      <c r="H14">
         <v>33.3333333333333</v>
       </c>
-      <c r="I13">
+      <c r="I14">
         <v>181777</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>32</v>
-      </c>
-      <c r="B14">
-        <v>64</v>
-      </c>
-      <c r="C14">
-        <v>512</v>
-      </c>
-      <c r="D14">
-        <v>37867</v>
-      </c>
-      <c r="E14">
-        <v>55760</v>
-      </c>
-      <c r="F14">
-        <v>2499</v>
-      </c>
-      <c r="G14" s="2">
-        <f t="shared" si="0"/>
-        <v>139.71944335773767</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>32</v>
       </c>
       <c r="B15">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="C15">
         <v>512</v>
       </c>
       <c r="D15">
+        <v>37867</v>
+      </c>
+      <c r="E15">
+        <v>55760</v>
+      </c>
+      <c r="F15">
+        <v>2499</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>139.71944335773767</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>32</v>
+      </c>
+      <c r="B16">
+        <v>16</v>
+      </c>
+      <c r="C16">
+        <v>512</v>
+      </c>
+      <c r="D16">
         <v>36893</v>
       </c>
-      <c r="E15">
+      <c r="E16">
         <v>54815</v>
       </c>
-      <c r="F15">
-        <v>2499</v>
-      </c>
-      <c r="G15" s="2">
+      <c r="F16">
+        <v>2499</v>
+      </c>
+      <c r="G16" s="2">
         <f t="shared" si="0"/>
         <v>139.49336011605848</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>32</v>
-      </c>
-      <c r="B16">
-        <v>128</v>
-      </c>
-      <c r="C16">
-        <v>128</v>
-      </c>
-      <c r="D16">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>32</v>
+      </c>
+      <c r="B17">
+        <v>128</v>
+      </c>
+      <c r="C17">
+        <v>128</v>
+      </c>
+      <c r="D17">
         <v>35704</v>
       </c>
-      <c r="E16">
+      <c r="E17">
         <v>53730</v>
       </c>
-      <c r="F16">
-        <v>2499</v>
-      </c>
-      <c r="G16" s="2">
+      <c r="F17">
+        <v>2499</v>
+      </c>
+      <c r="G17" s="2">
         <f t="shared" si="0"/>
         <v>138.68856096749141</v>
       </c>
-      <c r="H16">
+      <c r="H17">
         <v>33.3333333333333</v>
       </c>
-      <c r="I16">
+      <c r="I17">
         <v>90912</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>32</v>
-      </c>
-      <c r="B17">
-        <v>8</v>
-      </c>
-      <c r="C17">
-        <v>16</v>
-      </c>
-      <c r="D17">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>32</v>
+      </c>
+      <c r="B18">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>16</v>
+      </c>
+      <c r="D18">
         <v>39380</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <v>57418</v>
       </c>
-      <c r="F17">
-        <v>2499</v>
-      </c>
-      <c r="G17" s="2">
+      <c r="F18">
+        <v>2499</v>
+      </c>
+      <c r="G18" s="2">
         <f t="shared" si="0"/>
         <v>138.59629670695199</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>32</v>
-      </c>
-      <c r="B18">
-        <v>32</v>
-      </c>
-      <c r="C18">
-        <v>128</v>
-      </c>
-      <c r="D18">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>32</v>
+      </c>
+      <c r="B19">
+        <v>32</v>
+      </c>
+      <c r="C19">
+        <v>128</v>
+      </c>
+      <c r="D19">
         <v>38569</v>
       </c>
-      <c r="E18">
+      <c r="E19">
         <v>56617</v>
       </c>
-      <c r="F18">
-        <v>2499</v>
-      </c>
-      <c r="G18" s="2">
+      <c r="F19">
+        <v>2499</v>
+      </c>
+      <c r="G19" s="2">
         <f t="shared" si="0"/>
         <v>138.51950354609929</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>32</v>
-      </c>
-      <c r="B19">
-        <v>16</v>
-      </c>
-      <c r="C19">
-        <v>16</v>
-      </c>
-      <c r="D19">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>32</v>
+      </c>
+      <c r="B20">
+        <v>16</v>
+      </c>
+      <c r="C20">
+        <v>16</v>
+      </c>
+      <c r="D20">
         <v>38083</v>
       </c>
-      <c r="E19">
+      <c r="E20">
         <v>56159</v>
       </c>
-      <c r="F19">
-        <v>2499</v>
-      </c>
-      <c r="G19" s="2">
+      <c r="F20">
+        <v>2499</v>
+      </c>
+      <c r="G20" s="2">
         <f t="shared" si="0"/>
         <v>138.3049347200708</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>32</v>
-      </c>
-      <c r="B20">
-        <v>16</v>
-      </c>
-      <c r="C20">
-        <v>8</v>
-      </c>
-      <c r="D20">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>32</v>
+      </c>
+      <c r="B21">
+        <v>16</v>
+      </c>
+      <c r="C21">
+        <v>8</v>
+      </c>
+      <c r="D21">
         <v>37374</v>
       </c>
-      <c r="E20">
+      <c r="E21">
         <v>55536</v>
       </c>
-      <c r="F20">
-        <v>2499</v>
-      </c>
-      <c r="G20" s="2">
+      <c r="F21">
+        <v>2499</v>
+      </c>
+      <c r="G21" s="2">
         <f t="shared" si="0"/>
         <v>137.6500385420108</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>32</v>
-      </c>
-      <c r="B21">
-        <v>8</v>
-      </c>
-      <c r="C21">
-        <v>128</v>
-      </c>
-      <c r="D21">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>32</v>
+      </c>
+      <c r="B22">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>128</v>
+      </c>
+      <c r="D22">
         <v>38783</v>
       </c>
-      <c r="E21">
+      <c r="E22">
         <v>56967</v>
       </c>
-      <c r="F21">
-        <v>2499</v>
-      </c>
-      <c r="G21" s="2">
+      <c r="F22">
+        <v>2499</v>
+      </c>
+      <c r="G22" s="2">
         <f t="shared" si="0"/>
         <v>137.48350197976242</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>32</v>
-      </c>
-      <c r="B22">
-        <v>16</v>
-      </c>
-      <c r="C22">
-        <v>64</v>
-      </c>
-      <c r="D22">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>32</v>
+      </c>
+      <c r="B23">
+        <v>16</v>
+      </c>
+      <c r="C23">
+        <v>64</v>
+      </c>
+      <c r="D23">
         <v>38440</v>
       </c>
-      <c r="E22">
+      <c r="E23">
         <v>56714</v>
       </c>
-      <c r="F22">
-        <v>2499</v>
-      </c>
-      <c r="G22" s="2">
+      <c r="F23">
+        <v>2499</v>
+      </c>
+      <c r="G23" s="2">
         <f t="shared" si="0"/>
         <v>136.80639159461529</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>32</v>
-      </c>
-      <c r="B23">
-        <v>128</v>
-      </c>
-      <c r="C23">
-        <v>16</v>
-      </c>
-      <c r="D23">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>32</v>
+      </c>
+      <c r="B24">
+        <v>128</v>
+      </c>
+      <c r="C24">
+        <v>16</v>
+      </c>
+      <c r="D24">
         <v>40377</v>
       </c>
-      <c r="E23">
+      <c r="E24">
         <v>58654</v>
       </c>
-      <c r="F23">
-        <v>2499</v>
-      </c>
-      <c r="G23" s="2">
+      <c r="F24">
+        <v>2499</v>
+      </c>
+      <c r="G24" s="2">
         <f t="shared" si="0"/>
         <v>136.78393609454506</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>32</v>
-      </c>
-      <c r="B24">
-        <v>8</v>
-      </c>
-      <c r="C24">
-        <v>32</v>
-      </c>
-      <c r="D24">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>32</v>
+      </c>
+      <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>32</v>
+      </c>
+      <c r="D25">
         <v>39720</v>
       </c>
-      <c r="E24">
+      <c r="E25">
         <v>58025</v>
       </c>
-      <c r="F24">
-        <v>2499</v>
-      </c>
-      <c r="G24" s="2">
+      <c r="F25">
+        <v>2499</v>
+      </c>
+      <c r="G25" s="2">
         <f t="shared" si="0"/>
         <v>136.57470636438131</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>32</v>
-      </c>
-      <c r="B25">
-        <v>16</v>
-      </c>
-      <c r="C25">
-        <v>32</v>
-      </c>
-      <c r="D25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>32</v>
+      </c>
+      <c r="B26">
+        <v>16</v>
+      </c>
+      <c r="C26">
+        <v>32</v>
+      </c>
+      <c r="D26">
         <v>37638</v>
       </c>
-      <c r="E25">
+      <c r="E26">
         <v>55958</v>
       </c>
-      <c r="F25">
-        <v>2499</v>
-      </c>
-      <c r="G25" s="2">
+      <c r="F26">
+        <v>2499</v>
+      </c>
+      <c r="G26" s="2">
         <f t="shared" si="0"/>
         <v>136.46288209606988</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>32</v>
-      </c>
-      <c r="B26">
-        <v>256</v>
-      </c>
-      <c r="C26">
-        <v>128</v>
-      </c>
-      <c r="D26">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>32</v>
+      </c>
+      <c r="B27">
+        <v>256</v>
+      </c>
+      <c r="C27">
+        <v>128</v>
+      </c>
+      <c r="D27">
         <v>38370</v>
       </c>
-      <c r="E26">
+      <c r="E27">
         <v>56755</v>
       </c>
-      <c r="F26">
-        <v>2499</v>
-      </c>
-      <c r="G26" s="2">
+      <c r="F27">
+        <v>2499</v>
+      </c>
+      <c r="G27" s="2">
         <f t="shared" si="0"/>
         <v>135.98041881968999</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>32</v>
-      </c>
-      <c r="B27">
-        <v>256</v>
-      </c>
-      <c r="C27">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>32</v>
+      </c>
+      <c r="B28">
+        <v>256</v>
+      </c>
+      <c r="C28">
         <v>512</v>
       </c>
-      <c r="D27">
+      <c r="D28">
         <v>40463</v>
       </c>
-      <c r="E27">
+      <c r="E28">
         <v>58894</v>
       </c>
-      <c r="F27">
-        <v>2499</v>
-      </c>
-      <c r="G27" s="2">
+      <c r="F28">
+        <v>2499</v>
+      </c>
+      <c r="G28" s="2">
         <f t="shared" si="0"/>
         <v>135.64103955292714</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>32</v>
-      </c>
-      <c r="B28">
-        <v>8</v>
-      </c>
-      <c r="C28">
-        <v>8</v>
-      </c>
-      <c r="D28">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>32</v>
+      </c>
+      <c r="B29">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <v>8</v>
+      </c>
+      <c r="D29">
         <v>38832</v>
       </c>
-      <c r="E28">
+      <c r="E29">
         <v>57291</v>
       </c>
-      <c r="F28">
-        <v>2499</v>
-      </c>
-      <c r="G28" s="2">
+      <c r="F29">
+        <v>2499</v>
+      </c>
+      <c r="G29" s="2">
         <f t="shared" si="0"/>
         <v>135.43528901890679</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>32</v>
-      </c>
-      <c r="B29">
-        <v>8</v>
-      </c>
-      <c r="C29">
-        <v>64</v>
-      </c>
-      <c r="D29">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>32</v>
+      </c>
+      <c r="B30">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <v>64</v>
+      </c>
+      <c r="D30">
         <v>39372</v>
       </c>
-      <c r="E29">
+      <c r="E30">
         <v>57870</v>
       </c>
-      <c r="F29">
-        <v>2499</v>
-      </c>
-      <c r="G29" s="2">
+      <c r="F30">
+        <v>2499</v>
+      </c>
+      <c r="G30" s="2">
         <f t="shared" si="0"/>
         <v>135.14974591847766</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>32</v>
-      </c>
-      <c r="B30">
-        <v>8</v>
-      </c>
-      <c r="C30">
-        <v>256</v>
-      </c>
-      <c r="D30">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>32</v>
+      </c>
+      <c r="B31">
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <v>256</v>
+      </c>
+      <c r="D31">
         <v>38201</v>
       </c>
-      <c r="E30">
+      <c r="E31">
         <v>56737</v>
       </c>
-      <c r="F30">
-        <v>2499</v>
-      </c>
-      <c r="G30" s="2">
+      <c r="F31">
+        <v>2499</v>
+      </c>
+      <c r="G31" s="2">
         <f t="shared" si="0"/>
         <v>134.87268018990073</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>32</v>
-      </c>
-      <c r="B31">
-        <v>16</v>
-      </c>
-      <c r="C31">
-        <v>256</v>
-      </c>
-      <c r="D31">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>16</v>
+      </c>
+      <c r="C32">
+        <v>256</v>
+      </c>
+      <c r="D32">
         <v>37277</v>
       </c>
-      <c r="E31">
+      <c r="E32">
         <v>55846</v>
       </c>
-      <c r="F31">
-        <v>2499</v>
-      </c>
-      <c r="G31" s="2">
+      <c r="F32">
+        <v>2499</v>
+      </c>
+      <c r="G32" s="2">
         <f t="shared" si="0"/>
         <v>134.63299046798426</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>32</v>
-      </c>
-      <c r="B32">
-        <v>128</v>
-      </c>
-      <c r="C32">
-        <v>512</v>
-      </c>
-      <c r="D32">
-        <v>40032</v>
-      </c>
-      <c r="E32">
-        <v>58603</v>
-      </c>
-      <c r="F32">
-        <v>2499</v>
-      </c>
-      <c r="G32" s="2">
-        <f t="shared" si="0"/>
-        <v>134.61849119595067</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -10587,20 +10599,20 @@
         <v>128</v>
       </c>
       <c r="C33">
-        <v>256</v>
+        <v>512</v>
       </c>
       <c r="D33">
-        <v>40112</v>
+        <v>40032</v>
       </c>
       <c r="E33">
-        <v>58717</v>
+        <v>58603</v>
       </c>
       <c r="F33">
         <v>2499</v>
       </c>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G64" si="1">(1+F33)/(E33-D33)*1000</f>
-        <v>134.37248051599033</v>
+        <v>134.61849119595067</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -10611,20 +10623,20 @@
         <v>128</v>
       </c>
       <c r="C34">
-        <v>64</v>
+        <v>256</v>
       </c>
       <c r="D34">
-        <v>39632</v>
+        <v>40112</v>
       </c>
       <c r="E34">
-        <v>58245</v>
+        <v>58717</v>
       </c>
       <c r="F34">
         <v>2499</v>
       </c>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>134.31472626658785</v>
+        <v>134.37248051599033</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -10635,20 +10647,20 @@
         <v>128</v>
       </c>
       <c r="C35">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="D35">
-        <v>41123</v>
+        <v>39632</v>
       </c>
       <c r="E35">
-        <v>59745</v>
+        <v>58245</v>
       </c>
       <c r="F35">
         <v>2499</v>
       </c>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>134.24981205026313</v>
+        <v>134.31472626658785</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -10656,23 +10668,23 @@
         <v>32</v>
       </c>
       <c r="B36">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="C36">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="D36">
-        <v>39991</v>
+        <v>41123</v>
       </c>
       <c r="E36">
-        <v>58618</v>
+        <v>59745</v>
       </c>
       <c r="F36">
         <v>2499</v>
       </c>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>134.21377570193803</v>
+        <v>134.24981205026313</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -10683,20 +10695,20 @@
         <v>256</v>
       </c>
       <c r="C37">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="D37">
-        <v>40134</v>
+        <v>39991</v>
       </c>
       <c r="E37">
-        <v>58775</v>
+        <v>58618</v>
       </c>
       <c r="F37">
         <v>2499</v>
       </c>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
-        <v>134.11297677163242</v>
+        <v>134.21377570193803</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -10707,20 +10719,20 @@
         <v>256</v>
       </c>
       <c r="C38">
-        <v>256</v>
+        <v>32</v>
       </c>
       <c r="D38">
-        <v>40770</v>
+        <v>40134</v>
       </c>
       <c r="E38">
-        <v>59442</v>
+        <v>58775</v>
       </c>
       <c r="F38">
         <v>2499</v>
       </c>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
-        <v>133.89031705227077</v>
+        <v>134.11297677163242</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -10728,23 +10740,23 @@
         <v>32</v>
       </c>
       <c r="B39">
-        <v>16</v>
+        <v>256</v>
       </c>
       <c r="C39">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="D39">
-        <v>39351</v>
+        <v>40770</v>
       </c>
       <c r="E39">
-        <v>58461</v>
+        <v>59442</v>
       </c>
       <c r="F39">
         <v>2499</v>
       </c>
       <c r="G39" s="2">
         <f t="shared" si="1"/>
-        <v>130.82155939298795</v>
+        <v>133.89031705227077</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -10752,23 +10764,23 @@
         <v>32</v>
       </c>
       <c r="B40">
-        <v>128</v>
+        <v>16</v>
       </c>
       <c r="C40">
-        <v>8</v>
+        <v>128</v>
       </c>
       <c r="D40">
-        <v>41916</v>
+        <v>39351</v>
       </c>
       <c r="E40">
-        <v>61350</v>
+        <v>58461</v>
       </c>
       <c r="F40">
         <v>2499</v>
       </c>
       <c r="G40" s="2">
         <f t="shared" si="1"/>
-        <v>128.64052691159822</v>
+        <v>130.82155939298795</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -10776,47 +10788,47 @@
         <v>32</v>
       </c>
       <c r="B41">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="C41">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D41">
-        <v>40043</v>
+        <v>41916</v>
       </c>
       <c r="E41">
-        <v>60136</v>
+        <v>61350</v>
       </c>
       <c r="F41">
         <v>2499</v>
       </c>
       <c r="G41" s="2">
         <f t="shared" si="1"/>
-        <v>124.42144030259294</v>
+        <v>128.64052691159822</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="B42">
-        <v>32</v>
+        <v>256</v>
       </c>
       <c r="C42">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D42">
-        <v>53008</v>
+        <v>40043</v>
       </c>
       <c r="E42">
-        <v>76299</v>
+        <v>60136</v>
       </c>
       <c r="F42">
         <v>2499</v>
       </c>
       <c r="G42" s="2">
         <f t="shared" si="1"/>
-        <v>107.33759821390235</v>
+        <v>124.42144030259294</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -10827,20 +10839,20 @@
         <v>32</v>
       </c>
       <c r="C43">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D43">
-        <v>53845</v>
+        <v>53008</v>
       </c>
       <c r="E43">
-        <v>77320</v>
+        <v>76299</v>
       </c>
       <c r="F43">
         <v>2499</v>
       </c>
       <c r="G43" s="2">
         <f t="shared" si="1"/>
-        <v>106.49627263045794</v>
+        <v>107.33759821390235</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -10851,20 +10863,20 @@
         <v>32</v>
       </c>
       <c r="C44">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="D44">
-        <v>53562</v>
+        <v>53845</v>
       </c>
       <c r="E44">
-        <v>77215</v>
+        <v>77320</v>
       </c>
       <c r="F44">
         <v>2499</v>
       </c>
       <c r="G44" s="2">
         <f t="shared" si="1"/>
-        <v>105.69483786411872</v>
+        <v>106.49627263045794</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -10872,23 +10884,23 @@
         <v>16</v>
       </c>
       <c r="B45">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="C45">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="D45">
-        <v>55218</v>
+        <v>53562</v>
       </c>
       <c r="E45">
-        <v>78986</v>
+        <v>77215</v>
       </c>
       <c r="F45">
         <v>2499</v>
       </c>
       <c r="G45" s="2">
         <f t="shared" si="1"/>
-        <v>105.18343991921913</v>
+        <v>105.69483786411872</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -10896,23 +10908,23 @@
         <v>16</v>
       </c>
       <c r="B46">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="C46">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="D46">
-        <v>52577</v>
+        <v>55218</v>
       </c>
       <c r="E46">
-        <v>76385</v>
+        <v>78986</v>
       </c>
       <c r="F46">
         <v>2499</v>
       </c>
       <c r="G46" s="2">
         <f t="shared" si="1"/>
-        <v>105.00672043010753</v>
+        <v>105.18343991921913</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -10920,23 +10932,23 @@
         <v>16</v>
       </c>
       <c r="B47">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="C47">
         <v>256</v>
       </c>
       <c r="D47">
-        <v>55412</v>
+        <v>52577</v>
       </c>
       <c r="E47">
-        <v>79265</v>
+        <v>76385</v>
       </c>
       <c r="F47">
         <v>2499</v>
       </c>
       <c r="G47" s="2">
         <f t="shared" si="1"/>
-        <v>104.80861946086446</v>
+        <v>105.00672043010753</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -10947,20 +10959,20 @@
         <v>64</v>
       </c>
       <c r="C48">
-        <v>16</v>
+        <v>256</v>
       </c>
       <c r="D48">
-        <v>55654</v>
+        <v>55412</v>
       </c>
       <c r="E48">
-        <v>79610</v>
+        <v>79265</v>
       </c>
       <c r="F48">
         <v>2499</v>
       </c>
       <c r="G48" s="2">
         <f t="shared" si="1"/>
-        <v>104.35798964768743</v>
+        <v>104.80861946086446</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -10971,20 +10983,20 @@
         <v>64</v>
       </c>
       <c r="C49">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D49">
-        <v>56815</v>
+        <v>55654</v>
       </c>
       <c r="E49">
-        <v>80863</v>
+        <v>79610</v>
       </c>
       <c r="F49">
         <v>2499</v>
       </c>
       <c r="G49" s="2">
         <f t="shared" si="1"/>
-        <v>103.95874916833</v>
+        <v>104.35798964768743</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -10995,20 +11007,20 @@
         <v>64</v>
       </c>
       <c r="C50">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="D50">
-        <v>57253</v>
+        <v>56815</v>
       </c>
       <c r="E50">
-        <v>81410</v>
+        <v>80863</v>
       </c>
       <c r="F50">
         <v>2499</v>
       </c>
       <c r="G50" s="2">
         <f t="shared" si="1"/>
-        <v>103.48967173076127</v>
+        <v>103.95874916833</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -11016,23 +11028,23 @@
         <v>16</v>
       </c>
       <c r="B51">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="C51">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="D51">
-        <v>53279</v>
+        <v>57253</v>
       </c>
       <c r="E51">
-        <v>77570</v>
+        <v>81410</v>
       </c>
       <c r="F51">
         <v>2499</v>
       </c>
       <c r="G51" s="2">
         <f t="shared" si="1"/>
-        <v>102.91877650158494</v>
+        <v>103.48967173076127</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -11043,20 +11055,20 @@
         <v>32</v>
       </c>
       <c r="C52">
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="D52">
-        <v>56620</v>
+        <v>53279</v>
       </c>
       <c r="E52">
-        <v>81422</v>
+        <v>77570</v>
       </c>
       <c r="F52">
         <v>2499</v>
       </c>
       <c r="G52" s="2">
         <f t="shared" si="1"/>
-        <v>100.79832271591</v>
+        <v>102.91877650158494</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -11064,71 +11076,71 @@
         <v>16</v>
       </c>
       <c r="B53">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="C53">
-        <v>512</v>
+        <v>128</v>
       </c>
       <c r="D53">
-        <v>55762</v>
+        <v>56620</v>
       </c>
       <c r="E53">
-        <v>80610</v>
+        <v>81422</v>
       </c>
       <c r="F53">
         <v>2499</v>
       </c>
       <c r="G53" s="2">
         <f t="shared" si="1"/>
-        <v>100.6117192530586</v>
+        <v>100.79832271591</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B54">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="C54">
         <v>512</v>
       </c>
       <c r="D54">
-        <v>38586</v>
+        <v>55762</v>
       </c>
       <c r="E54">
-        <v>63439</v>
+        <v>80610</v>
       </c>
       <c r="F54">
         <v>2499</v>
       </c>
       <c r="G54" s="2">
         <f t="shared" si="1"/>
-        <v>100.59147788999316</v>
+        <v>100.6117192530586</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="B55">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="C55">
         <v>512</v>
       </c>
       <c r="D55">
-        <v>53132</v>
+        <v>38586</v>
       </c>
       <c r="E55">
-        <v>78039</v>
+        <v>63439</v>
       </c>
       <c r="F55">
         <v>2499</v>
       </c>
       <c r="G55" s="2">
         <f t="shared" si="1"/>
-        <v>100.37338900710644</v>
+        <v>100.59147788999316</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -11136,23 +11148,23 @@
         <v>16</v>
       </c>
       <c r="B56">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="C56">
-        <v>8</v>
+        <v>512</v>
       </c>
       <c r="D56">
-        <v>55539</v>
+        <v>53132</v>
       </c>
       <c r="E56">
-        <v>80661</v>
+        <v>78039</v>
       </c>
       <c r="F56">
         <v>2499</v>
       </c>
       <c r="G56" s="2">
         <f t="shared" si="1"/>
-        <v>99.514369875009947</v>
+        <v>100.37338900710644</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -11163,20 +11175,20 @@
         <v>16</v>
       </c>
       <c r="C57">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D57">
-        <v>56161</v>
+        <v>55539</v>
       </c>
       <c r="E57">
-        <v>81424</v>
+        <v>80661</v>
       </c>
       <c r="F57">
         <v>2499</v>
       </c>
       <c r="G57" s="2">
         <f t="shared" si="1"/>
-        <v>98.958951826782254</v>
+        <v>99.514369875009947</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -11187,20 +11199,20 @@
         <v>16</v>
       </c>
       <c r="C58">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="D58">
-        <v>56717</v>
+        <v>56161</v>
       </c>
       <c r="E58">
-        <v>82120</v>
+        <v>81424</v>
       </c>
       <c r="F58">
         <v>2499</v>
       </c>
       <c r="G58" s="2">
         <f t="shared" si="1"/>
-        <v>98.413573200015747</v>
+        <v>98.958951826782254</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -11211,20 +11223,20 @@
         <v>16</v>
       </c>
       <c r="C59">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="D59">
-        <v>55961</v>
+        <v>56717</v>
       </c>
       <c r="E59">
-        <v>81453</v>
+        <v>82120</v>
       </c>
       <c r="F59">
         <v>2499</v>
       </c>
       <c r="G59" s="2">
         <f t="shared" si="1"/>
-        <v>98.069982739683041</v>
+        <v>98.413573200015747</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -11232,23 +11244,23 @@
         <v>16</v>
       </c>
       <c r="B60">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="C60">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="D60">
-        <v>56186</v>
+        <v>55961</v>
       </c>
       <c r="E60">
-        <v>81938</v>
+        <v>81453</v>
       </c>
       <c r="F60">
         <v>2499</v>
       </c>
       <c r="G60" s="2">
         <f t="shared" si="1"/>
-        <v>97.079838459148803</v>
+        <v>98.069982739683041</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -11256,23 +11268,23 @@
         <v>16</v>
       </c>
       <c r="B61">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C61">
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="D61">
-        <v>53732</v>
+        <v>56186</v>
       </c>
       <c r="E61">
-        <v>80038</v>
+        <v>81938</v>
       </c>
       <c r="F61">
         <v>2499</v>
       </c>
       <c r="G61" s="2">
         <f t="shared" si="1"/>
-        <v>95.035353151372306</v>
+        <v>97.079838459148803</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -11280,23 +11292,23 @@
         <v>16</v>
       </c>
       <c r="B62">
-        <v>16</v>
+        <v>128</v>
       </c>
       <c r="C62">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="D62">
-        <v>55848</v>
+        <v>53732</v>
       </c>
       <c r="E62">
-        <v>82180</v>
+        <v>80038</v>
       </c>
       <c r="F62">
         <v>2499</v>
       </c>
       <c r="G62" s="2">
         <f t="shared" si="1"/>
-        <v>94.941516026127914</v>
+        <v>95.035353151372306</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -11307,20 +11319,20 @@
         <v>16</v>
       </c>
       <c r="C63">
-        <v>512</v>
+        <v>256</v>
       </c>
       <c r="D63">
-        <v>54818</v>
+        <v>55848</v>
       </c>
       <c r="E63">
-        <v>81280</v>
+        <v>82180</v>
       </c>
       <c r="F63">
         <v>2499</v>
       </c>
       <c r="G63" s="2">
         <f t="shared" si="1"/>
-        <v>94.475096364598286</v>
+        <v>94.941516026127914</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -11331,20 +11343,20 @@
         <v>16</v>
       </c>
       <c r="C64">
-        <v>128</v>
+        <v>512</v>
       </c>
       <c r="D64">
-        <v>58464</v>
+        <v>54818</v>
       </c>
       <c r="E64">
-        <v>85107</v>
+        <v>81280</v>
       </c>
       <c r="F64">
         <v>2499</v>
       </c>
       <c r="G64" s="2">
         <f t="shared" si="1"/>
-        <v>93.833277033367111</v>
+        <v>94.475096364598286</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -11352,23 +11364,23 @@
         <v>16</v>
       </c>
       <c r="B65">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C65">
-        <v>32</v>
+        <v>128</v>
       </c>
       <c r="D65">
-        <v>58027</v>
+        <v>58464</v>
       </c>
       <c r="E65">
-        <v>84681</v>
+        <v>85107</v>
       </c>
       <c r="F65">
         <v>2499</v>
       </c>
       <c r="G65" s="2">
         <f t="shared" ref="G65:G96" si="2">(1+F65)/(E65-D65)*1000</f>
-        <v>93.794552412395888</v>
+        <v>93.833277033367111</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -11379,20 +11391,20 @@
         <v>8</v>
       </c>
       <c r="C66">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="D66">
-        <v>57294</v>
+        <v>58027</v>
       </c>
       <c r="E66">
-        <v>83976</v>
+        <v>84681</v>
       </c>
       <c r="F66">
         <v>2499</v>
       </c>
       <c r="G66" s="2">
         <f t="shared" si="2"/>
-        <v>93.696124728281234</v>
+        <v>93.794552412395888</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -11403,20 +11415,20 @@
         <v>8</v>
       </c>
       <c r="C67">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D67">
-        <v>57422</v>
+        <v>57294</v>
       </c>
       <c r="E67">
-        <v>84108</v>
+        <v>83976</v>
       </c>
       <c r="F67">
         <v>2499</v>
       </c>
       <c r="G67" s="2">
         <f t="shared" si="2"/>
-        <v>93.682080491643561</v>
+        <v>93.696124728281234</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -11424,23 +11436,23 @@
         <v>16</v>
       </c>
       <c r="B68">
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="C68">
         <v>16</v>
       </c>
       <c r="D68">
-        <v>58657</v>
+        <v>57422</v>
       </c>
       <c r="E68">
-        <v>85351</v>
+        <v>84108</v>
       </c>
       <c r="F68">
         <v>2499</v>
       </c>
       <c r="G68" s="2">
         <f t="shared" si="2"/>
-        <v>93.654004645238629</v>
+        <v>93.682080491643561</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -11448,23 +11460,23 @@
         <v>16</v>
       </c>
       <c r="B69">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="C69">
-        <v>512</v>
+        <v>16</v>
       </c>
       <c r="D69">
-        <v>58897</v>
+        <v>58657</v>
       </c>
       <c r="E69">
-        <v>85627</v>
+        <v>85351</v>
       </c>
       <c r="F69">
         <v>2499</v>
       </c>
       <c r="G69" s="2">
         <f t="shared" si="2"/>
-        <v>93.527871305649086</v>
+        <v>93.654004645238629</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -11475,20 +11487,20 @@
         <v>256</v>
       </c>
       <c r="C70">
-        <v>256</v>
+        <v>512</v>
       </c>
       <c r="D70">
-        <v>59446</v>
+        <v>58897</v>
       </c>
       <c r="E70">
-        <v>86208</v>
+        <v>85627</v>
       </c>
       <c r="F70">
         <v>2499</v>
       </c>
       <c r="G70" s="2">
         <f t="shared" si="2"/>
-        <v>93.41603766534638</v>
+        <v>93.527871305649086</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -11496,23 +11508,23 @@
         <v>16</v>
       </c>
       <c r="B71">
-        <v>8</v>
+        <v>256</v>
       </c>
       <c r="C71">
         <v>256</v>
       </c>
       <c r="D71">
-        <v>56741</v>
+        <v>59446</v>
       </c>
       <c r="E71">
-        <v>83566</v>
+        <v>86208</v>
       </c>
       <c r="F71">
         <v>2499</v>
       </c>
       <c r="G71" s="2">
         <f t="shared" si="2"/>
-        <v>93.196644920782845</v>
+        <v>93.41603766534638</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -11520,23 +11532,23 @@
         <v>16</v>
       </c>
       <c r="B72">
-        <v>256</v>
+        <v>8</v>
       </c>
       <c r="C72">
-        <v>64</v>
+        <v>256</v>
       </c>
       <c r="D72">
-        <v>58620</v>
+        <v>56741</v>
       </c>
       <c r="E72">
-        <v>85482</v>
+        <v>83566</v>
       </c>
       <c r="F72">
         <v>2499</v>
       </c>
       <c r="G72" s="2">
         <f t="shared" si="2"/>
-        <v>93.068274886456706</v>
+        <v>93.196644920782845</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -11544,23 +11556,23 @@
         <v>16</v>
       </c>
       <c r="B73">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="C73">
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="D73">
-        <v>58607</v>
+        <v>58620</v>
       </c>
       <c r="E73">
-        <v>85504</v>
+        <v>85482</v>
       </c>
       <c r="F73">
         <v>2499</v>
       </c>
       <c r="G73" s="2">
         <f t="shared" si="2"/>
-        <v>92.947168829237469</v>
+        <v>93.068274886456706</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -11571,20 +11583,20 @@
         <v>128</v>
       </c>
       <c r="C74">
-        <v>32</v>
+        <v>512</v>
       </c>
       <c r="D74">
-        <v>59748</v>
+        <v>58607</v>
       </c>
       <c r="E74">
-        <v>86664</v>
+        <v>85504</v>
       </c>
       <c r="F74">
         <v>2499</v>
       </c>
       <c r="G74" s="2">
         <f t="shared" si="2"/>
-        <v>92.881557437955124</v>
+        <v>92.947168829237469</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -11592,23 +11604,23 @@
         <v>16</v>
       </c>
       <c r="B75">
-        <v>8</v>
+        <v>128</v>
       </c>
       <c r="C75">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="D75">
-        <v>56970</v>
+        <v>59748</v>
       </c>
       <c r="E75">
-        <v>83890</v>
+        <v>86664</v>
       </c>
       <c r="F75">
         <v>2499</v>
       </c>
       <c r="G75" s="2">
         <f t="shared" si="2"/>
-        <v>92.867756315007426</v>
+        <v>92.881557437955124</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -11616,23 +11628,23 @@
         <v>16</v>
       </c>
       <c r="B76">
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="C76">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="D76">
-        <v>58720</v>
+        <v>56970</v>
       </c>
       <c r="E76">
-        <v>85671</v>
+        <v>83890</v>
       </c>
       <c r="F76">
         <v>2499</v>
       </c>
       <c r="G76" s="2">
         <f t="shared" si="2"/>
-        <v>92.76093651441505</v>
+        <v>92.867756315007426</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -11640,23 +11652,23 @@
         <v>16</v>
       </c>
       <c r="B77">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="C77">
-        <v>32</v>
+        <v>256</v>
       </c>
       <c r="D77">
-        <v>58779</v>
+        <v>58720</v>
       </c>
       <c r="E77">
-        <v>85857</v>
+        <v>85671</v>
       </c>
       <c r="F77">
         <v>2499</v>
       </c>
       <c r="G77" s="2">
         <f t="shared" si="2"/>
-        <v>92.325873402762397</v>
+        <v>92.76093651441505</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -11664,23 +11676,23 @@
         <v>16</v>
       </c>
       <c r="B78">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="C78">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="D78">
-        <v>61353</v>
+        <v>58779</v>
       </c>
       <c r="E78">
-        <v>88435</v>
+        <v>85857</v>
       </c>
       <c r="F78">
         <v>2499</v>
       </c>
       <c r="G78" s="2">
         <f t="shared" si="2"/>
-        <v>92.312236910124795</v>
+        <v>92.325873402762397</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -11688,23 +11700,23 @@
         <v>16</v>
       </c>
       <c r="B79">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="C79">
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="D79">
-        <v>56757</v>
+        <v>61353</v>
       </c>
       <c r="E79">
-        <v>83848</v>
+        <v>88435</v>
       </c>
       <c r="F79">
         <v>2499</v>
       </c>
       <c r="G79" s="2">
         <f t="shared" si="2"/>
-        <v>92.281569524934483</v>
+        <v>92.312236910124795</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -11712,23 +11724,23 @@
         <v>16</v>
       </c>
       <c r="B80">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="C80">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="D80">
-        <v>58247</v>
+        <v>56757</v>
       </c>
       <c r="E80">
-        <v>85850</v>
+        <v>83848</v>
       </c>
       <c r="F80">
         <v>2499</v>
       </c>
       <c r="G80" s="2">
         <f t="shared" si="2"/>
-        <v>90.569865594319452</v>
+        <v>92.281569524934483</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -11736,23 +11748,23 @@
         <v>16</v>
       </c>
       <c r="B81">
-        <v>8</v>
+        <v>128</v>
       </c>
       <c r="C81">
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="D81">
-        <v>63445</v>
+        <v>58247</v>
       </c>
       <c r="E81">
-        <v>91349</v>
+        <v>85850</v>
       </c>
       <c r="F81">
         <v>2499</v>
       </c>
       <c r="G81" s="2">
         <f t="shared" si="2"/>
-        <v>89.592889908256879</v>
+        <v>90.569865594319452</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -11763,20 +11775,20 @@
         <v>8</v>
       </c>
       <c r="C82">
-        <v>64</v>
+        <v>512</v>
       </c>
       <c r="D82">
-        <v>57872</v>
+        <v>63445</v>
       </c>
       <c r="E82">
-        <v>86454</v>
+        <v>91349</v>
       </c>
       <c r="F82">
         <v>2499</v>
       </c>
       <c r="G82" s="2">
         <f t="shared" si="2"/>
-        <v>87.467636974319504</v>
+        <v>89.592889908256879</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -11784,47 +11796,47 @@
         <v>16</v>
       </c>
       <c r="B83">
-        <v>256</v>
+        <v>8</v>
       </c>
       <c r="C83">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="D83">
-        <v>60139</v>
+        <v>57872</v>
       </c>
       <c r="E83">
-        <v>89361</v>
+        <v>86454</v>
       </c>
       <c r="F83">
         <v>2499</v>
       </c>
       <c r="G83" s="2">
         <f t="shared" si="2"/>
-        <v>85.551981383888844</v>
+        <v>87.467636974319504</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B84">
-        <v>32</v>
+        <v>256</v>
       </c>
       <c r="C84">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D84">
-        <v>76302</v>
+        <v>60139</v>
       </c>
       <c r="E84">
-        <v>106618</v>
+        <v>89361</v>
       </c>
       <c r="F84">
         <v>2499</v>
       </c>
       <c r="G84" s="2">
         <f t="shared" si="2"/>
-        <v>82.464705106214538</v>
+        <v>85.551981383888844</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -11835,20 +11847,20 @@
         <v>32</v>
       </c>
       <c r="C85">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="D85">
-        <v>77217</v>
+        <v>76302</v>
       </c>
       <c r="E85">
-        <v>107539</v>
+        <v>106618</v>
       </c>
       <c r="F85">
         <v>2499</v>
       </c>
       <c r="G85" s="2">
         <f t="shared" si="2"/>
-        <v>82.448387309544216</v>
+        <v>82.464705106214538</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -11859,20 +11871,20 @@
         <v>32</v>
       </c>
       <c r="C86">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="D86">
-        <v>77572</v>
+        <v>77217</v>
       </c>
       <c r="E86">
-        <v>108269</v>
+        <v>107539</v>
       </c>
       <c r="F86">
         <v>2499</v>
       </c>
       <c r="G86" s="2">
         <f t="shared" si="2"/>
-        <v>81.441183177509203</v>
+        <v>82.448387309544216</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -11883,20 +11895,20 @@
         <v>32</v>
       </c>
       <c r="C87">
-        <v>256</v>
+        <v>8</v>
       </c>
       <c r="D87">
-        <v>76388</v>
+        <v>77572</v>
       </c>
       <c r="E87">
-        <v>107300</v>
+        <v>108269</v>
       </c>
       <c r="F87">
         <v>2499</v>
       </c>
       <c r="G87" s="2">
         <f t="shared" si="2"/>
-        <v>80.874741200828154</v>
+        <v>81.441183177509203</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -11907,20 +11919,20 @@
         <v>32</v>
       </c>
       <c r="C88">
-        <v>16</v>
+        <v>256</v>
       </c>
       <c r="D88">
-        <v>77324</v>
+        <v>76388</v>
       </c>
       <c r="E88">
-        <v>108291</v>
+        <v>107300</v>
       </c>
       <c r="F88">
         <v>2499</v>
       </c>
       <c r="G88" s="2">
         <f t="shared" si="2"/>
-        <v>80.731100849291181</v>
+        <v>80.874741200828154</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -11928,23 +11940,23 @@
         <v>8</v>
       </c>
       <c r="B89">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="C89">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D89">
-        <v>80865</v>
+        <v>77324</v>
       </c>
       <c r="E89">
-        <v>112237</v>
+        <v>108291</v>
       </c>
       <c r="F89">
         <v>2499</v>
       </c>
       <c r="G89" s="2">
         <f t="shared" si="2"/>
-        <v>79.688894555654727</v>
+        <v>80.731100849291181</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -11952,23 +11964,23 @@
         <v>8</v>
       </c>
       <c r="B90">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="C90">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="D90">
-        <v>81424</v>
+        <v>80865</v>
       </c>
       <c r="E90">
-        <v>112914</v>
+        <v>112237</v>
       </c>
       <c r="F90">
         <v>2499</v>
       </c>
       <c r="G90" s="2">
         <f t="shared" si="2"/>
-        <v>79.390282629406158</v>
+        <v>79.688894555654727</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -11976,23 +11988,23 @@
         <v>8</v>
       </c>
       <c r="B91">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="C91">
-        <v>16</v>
+        <v>128</v>
       </c>
       <c r="D91">
-        <v>79613</v>
+        <v>81424</v>
       </c>
       <c r="E91">
-        <v>111118</v>
+        <v>112914</v>
       </c>
       <c r="F91">
         <v>2499</v>
       </c>
       <c r="G91" s="2">
         <f t="shared" si="2"/>
-        <v>79.352483732740836</v>
+        <v>79.390282629406158</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -12003,20 +12015,20 @@
         <v>64</v>
       </c>
       <c r="C92">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="D92">
-        <v>81412</v>
+        <v>79613</v>
       </c>
       <c r="E92">
-        <v>113156</v>
+        <v>111118</v>
       </c>
       <c r="F92">
         <v>2499</v>
       </c>
       <c r="G92" s="2">
         <f t="shared" si="2"/>
-        <v>78.755040322580641</v>
+        <v>79.352483732740836</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -12024,23 +12036,23 @@
         <v>8</v>
       </c>
       <c r="B93">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="C93">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="D93">
-        <v>81456</v>
+        <v>81412</v>
       </c>
       <c r="E93">
-        <v>113210</v>
+        <v>113156</v>
       </c>
       <c r="F93">
         <v>2499</v>
       </c>
       <c r="G93" s="2">
         <f t="shared" si="2"/>
-        <v>78.730238710083768</v>
+        <v>78.755040322580641</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -12051,20 +12063,20 @@
         <v>16</v>
       </c>
       <c r="C94">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="D94">
-        <v>80663</v>
+        <v>81456</v>
       </c>
       <c r="E94">
-        <v>112485</v>
+        <v>113210</v>
       </c>
       <c r="F94">
         <v>2499</v>
       </c>
       <c r="G94" s="2">
         <f t="shared" si="2"/>
-        <v>78.562001131292817</v>
+        <v>78.730238710083768</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -12072,16 +12084,16 @@
         <v>8</v>
       </c>
       <c r="B95">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="C95">
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="D95">
-        <v>78989</v>
+        <v>80663</v>
       </c>
       <c r="E95">
-        <v>110811</v>
+        <v>112485</v>
       </c>
       <c r="F95">
         <v>2499</v>
@@ -12096,23 +12108,23 @@
         <v>8</v>
       </c>
       <c r="B96">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="C96">
-        <v>512</v>
+        <v>128</v>
       </c>
       <c r="D96">
-        <v>78042</v>
+        <v>78989</v>
       </c>
       <c r="E96">
-        <v>110099</v>
+        <v>110811</v>
       </c>
       <c r="F96">
         <v>2499</v>
       </c>
       <c r="G96" s="2">
         <f t="shared" si="2"/>
-        <v>77.986087282028876</v>
+        <v>78.562001131292817</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -12120,23 +12132,23 @@
         <v>8</v>
       </c>
       <c r="B97">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="C97">
-        <v>64</v>
+        <v>512</v>
       </c>
       <c r="D97">
-        <v>82122</v>
+        <v>78042</v>
       </c>
       <c r="E97">
-        <v>114383</v>
+        <v>110099</v>
       </c>
       <c r="F97">
         <v>2499</v>
       </c>
       <c r="G97" s="2">
-        <f t="shared" ref="G97:G127" si="3">(1+F97)/(E97-D97)*1000</f>
-        <v>77.492948141719097</v>
+        <f t="shared" ref="G97:G128" si="3">(1+F97)/(E97-D97)*1000</f>
+        <v>77.986087282028876</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -12147,20 +12159,20 @@
         <v>16</v>
       </c>
       <c r="C98">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="D98">
-        <v>81426</v>
+        <v>82122</v>
       </c>
       <c r="E98">
-        <v>113848</v>
+        <v>114383</v>
       </c>
       <c r="F98">
         <v>2499</v>
       </c>
       <c r="G98" s="2">
         <f t="shared" si="3"/>
-        <v>77.108136450558263</v>
+        <v>77.492948141719097</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -12168,23 +12180,23 @@
         <v>8</v>
       </c>
       <c r="B99">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="C99">
-        <v>256</v>
+        <v>16</v>
       </c>
       <c r="D99">
-        <v>79267</v>
+        <v>81426</v>
       </c>
       <c r="E99">
-        <v>112019</v>
+        <v>113848</v>
       </c>
       <c r="F99">
         <v>2499</v>
       </c>
       <c r="G99" s="2">
         <f t="shared" si="3"/>
-        <v>76.331216414264787</v>
+        <v>77.108136450558263</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -12192,23 +12204,23 @@
         <v>8</v>
       </c>
       <c r="B100">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="C100">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="D100">
-        <v>85109</v>
+        <v>79267</v>
       </c>
       <c r="E100">
-        <v>118244</v>
+        <v>112019</v>
       </c>
       <c r="F100">
         <v>2499</v>
       </c>
       <c r="G100" s="2">
         <f t="shared" si="3"/>
-        <v>75.448921080428562</v>
+        <v>76.331216414264787</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -12219,20 +12231,20 @@
         <v>16</v>
       </c>
       <c r="C101">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="D101">
-        <v>82182</v>
+        <v>85109</v>
       </c>
       <c r="E101">
-        <v>115688</v>
+        <v>118244</v>
       </c>
       <c r="F101">
         <v>2499</v>
       </c>
       <c r="G101" s="2">
         <f t="shared" si="3"/>
-        <v>74.61350205933266</v>
+        <v>75.448921080428562</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -12240,23 +12252,23 @@
         <v>8</v>
       </c>
       <c r="B102">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C102">
-        <v>16</v>
+        <v>256</v>
       </c>
       <c r="D102">
-        <v>84111</v>
+        <v>82182</v>
       </c>
       <c r="E102">
-        <v>117877</v>
+        <v>115688</v>
       </c>
       <c r="F102">
         <v>2499</v>
       </c>
       <c r="G102" s="2">
         <f t="shared" si="3"/>
-        <v>74.038974115974654</v>
+        <v>74.61350205933266</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -12267,20 +12279,20 @@
         <v>8</v>
       </c>
       <c r="C103">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D103">
-        <v>84683</v>
+        <v>84111</v>
       </c>
       <c r="E103">
-        <v>118511</v>
+        <v>117877</v>
       </c>
       <c r="F103">
         <v>2499</v>
       </c>
       <c r="G103" s="2">
         <f t="shared" si="3"/>
-        <v>73.903275393165416</v>
+        <v>74.038974115974654</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -12291,20 +12303,20 @@
         <v>8</v>
       </c>
       <c r="C104">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="D104">
-        <v>83978</v>
+        <v>84683</v>
       </c>
       <c r="E104">
-        <v>118101</v>
+        <v>118511</v>
       </c>
       <c r="F104">
         <v>2499</v>
       </c>
       <c r="G104" s="2">
         <f t="shared" si="3"/>
-        <v>73.264367142396623</v>
+        <v>73.903275393165416</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -12312,23 +12324,23 @@
         <v>8</v>
       </c>
       <c r="B105">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="C105">
-        <v>512</v>
+        <v>8</v>
       </c>
       <c r="D105">
-        <v>80612</v>
+        <v>83978</v>
       </c>
       <c r="E105">
-        <v>114760</v>
+        <v>118101</v>
       </c>
       <c r="F105">
         <v>2499</v>
       </c>
       <c r="G105" s="2">
         <f t="shared" si="3"/>
-        <v>73.210729764554301</v>
+        <v>73.264367142396623</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -12336,23 +12348,23 @@
         <v>8</v>
       </c>
       <c r="B106">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="C106">
-        <v>128</v>
+        <v>512</v>
       </c>
       <c r="D106">
-        <v>83892</v>
+        <v>80612</v>
       </c>
       <c r="E106">
-        <v>118300</v>
+        <v>114760</v>
       </c>
       <c r="F106">
         <v>2499</v>
       </c>
       <c r="G106" s="2">
         <f t="shared" si="3"/>
-        <v>72.657521506626367</v>
+        <v>73.210729764554301</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -12360,23 +12372,23 @@
         <v>8</v>
       </c>
       <c r="B107">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="C107">
-        <v>8</v>
+        <v>128</v>
       </c>
       <c r="D107">
-        <v>81940</v>
+        <v>83892</v>
       </c>
       <c r="E107">
-        <v>116526</v>
+        <v>118300</v>
       </c>
       <c r="F107">
         <v>2499</v>
       </c>
       <c r="G107" s="2">
         <f t="shared" si="3"/>
-        <v>72.283582952639804</v>
+        <v>72.657521506626367</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -12384,23 +12396,23 @@
         <v>8</v>
       </c>
       <c r="B108">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="C108">
-        <v>512</v>
+        <v>8</v>
       </c>
       <c r="D108">
-        <v>81284</v>
+        <v>81940</v>
       </c>
       <c r="E108">
-        <v>115969</v>
+        <v>116526</v>
       </c>
       <c r="F108">
         <v>2499</v>
       </c>
       <c r="G108" s="2">
         <f t="shared" si="3"/>
-        <v>72.077266830041793</v>
+        <v>72.283582952639804</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -12408,23 +12420,23 @@
         <v>8</v>
       </c>
       <c r="B109">
-        <v>128</v>
+        <v>16</v>
       </c>
       <c r="C109">
-        <v>16</v>
+        <v>512</v>
       </c>
       <c r="D109">
-        <v>85354</v>
+        <v>81284</v>
       </c>
       <c r="E109">
-        <v>120219</v>
+        <v>115969</v>
       </c>
       <c r="F109">
         <v>2499</v>
       </c>
       <c r="G109" s="2">
         <f t="shared" si="3"/>
-        <v>71.705148429657257</v>
+        <v>72.077266830041793</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -12435,20 +12447,20 @@
         <v>128</v>
       </c>
       <c r="C110">
-        <v>128</v>
+        <v>16</v>
       </c>
       <c r="D110">
-        <v>80041</v>
+        <v>85354</v>
       </c>
       <c r="E110">
-        <v>114959</v>
+        <v>120219</v>
       </c>
       <c r="F110">
         <v>2499</v>
       </c>
       <c r="G110" s="2">
         <f t="shared" si="3"/>
-        <v>71.596311358038832</v>
+        <v>71.705148429657257</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -12456,23 +12468,23 @@
         <v>8</v>
       </c>
       <c r="B111">
-        <v>8</v>
+        <v>128</v>
       </c>
       <c r="C111">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="D111">
-        <v>83568</v>
+        <v>80041</v>
       </c>
       <c r="E111">
-        <v>118718</v>
+        <v>114959</v>
       </c>
       <c r="F111">
         <v>2499</v>
       </c>
       <c r="G111" s="2">
         <f t="shared" si="3"/>
-        <v>71.123755334281654</v>
+        <v>71.596311358038832</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -12480,23 +12492,23 @@
         <v>8</v>
       </c>
       <c r="B112">
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="C112">
-        <v>8</v>
+        <v>256</v>
       </c>
       <c r="D112">
-        <v>88438</v>
+        <v>83568</v>
       </c>
       <c r="E112">
-        <v>123601</v>
+        <v>118718</v>
       </c>
       <c r="F112">
         <v>2499</v>
       </c>
       <c r="G112" s="2">
         <f t="shared" si="3"/>
-        <v>71.09746039871456</v>
+        <v>71.123755334281654</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -12504,23 +12516,23 @@
         <v>8</v>
       </c>
       <c r="B113">
-        <v>8</v>
+        <v>128</v>
       </c>
       <c r="C113">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="D113">
-        <v>86458</v>
+        <v>88438</v>
       </c>
       <c r="E113">
-        <v>121700</v>
+        <v>123601</v>
       </c>
       <c r="F113">
         <v>2499</v>
       </c>
       <c r="G113" s="2">
         <f t="shared" si="3"/>
-        <v>70.938085239203218</v>
+        <v>71.09746039871456</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -12531,20 +12543,20 @@
         <v>8</v>
       </c>
       <c r="C114">
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="D114">
-        <v>91352</v>
+        <v>86458</v>
       </c>
       <c r="E114">
-        <v>126600</v>
+        <v>121700</v>
       </c>
       <c r="F114">
         <v>2499</v>
       </c>
       <c r="G114" s="2">
         <f t="shared" si="3"/>
-        <v>70.926009986382212</v>
+        <v>70.938085239203218</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -12552,23 +12564,23 @@
         <v>8</v>
       </c>
       <c r="B115">
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="C115">
-        <v>256</v>
+        <v>512</v>
       </c>
       <c r="D115">
-        <v>85673</v>
+        <v>91352</v>
       </c>
       <c r="E115">
-        <v>121051</v>
+        <v>126600</v>
       </c>
       <c r="F115">
         <v>2499</v>
       </c>
       <c r="G115" s="2">
         <f t="shared" si="3"/>
-        <v>70.665385267680492</v>
+        <v>70.926009986382212</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -12579,20 +12591,20 @@
         <v>128</v>
       </c>
       <c r="C116">
-        <v>32</v>
+        <v>256</v>
       </c>
       <c r="D116">
-        <v>86668</v>
+        <v>85673</v>
       </c>
       <c r="E116">
-        <v>122163</v>
+        <v>121051</v>
       </c>
       <c r="F116">
         <v>2499</v>
       </c>
       <c r="G116" s="2">
         <f t="shared" si="3"/>
-        <v>70.432455275390893</v>
+        <v>70.665385267680492</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -12603,20 +12615,20 @@
         <v>128</v>
       </c>
       <c r="C117">
-        <v>512</v>
+        <v>32</v>
       </c>
       <c r="D117">
-        <v>85509</v>
+        <v>86668</v>
       </c>
       <c r="E117">
-        <v>121011</v>
+        <v>122163</v>
       </c>
       <c r="F117">
         <v>2499</v>
       </c>
       <c r="G117" s="2">
         <f t="shared" si="3"/>
-        <v>70.41856796800181</v>
+        <v>70.432455275390893</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -12627,37 +12639,37 @@
         <v>128</v>
       </c>
       <c r="C118">
-        <v>64</v>
+        <v>512</v>
       </c>
       <c r="D118">
-        <v>85852</v>
+        <v>85509</v>
       </c>
       <c r="E118">
-        <v>121712</v>
+        <v>121011</v>
       </c>
       <c r="F118">
         <v>2499</v>
       </c>
       <c r="G118" s="2">
         <f t="shared" si="3"/>
-        <v>69.715560513106524</v>
+        <v>70.41856796800181</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="B119">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="C119">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="D119">
-        <v>40347</v>
+        <v>85852</v>
       </c>
       <c r="E119">
-        <v>76207</v>
+        <v>121712</v>
       </c>
       <c r="F119">
         <v>2499</v>
@@ -12669,7 +12681,7 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="B120">
         <v>256</v>
@@ -12678,41 +12690,41 @@
         <v>8</v>
       </c>
       <c r="D120">
-        <v>76218</v>
+        <v>40347</v>
       </c>
       <c r="E120">
-        <v>113809</v>
+        <v>76207</v>
       </c>
       <c r="F120">
         <v>2499</v>
       </c>
       <c r="G120" s="2">
         <f t="shared" si="3"/>
-        <v>66.505280519273242</v>
+        <v>69.715560513106524</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B121">
         <v>256</v>
       </c>
       <c r="C121">
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="D121">
-        <v>83851</v>
+        <v>76218</v>
       </c>
       <c r="E121">
-        <v>124747</v>
+        <v>113809</v>
       </c>
       <c r="F121">
         <v>2499</v>
       </c>
       <c r="G121" s="2">
         <f t="shared" si="3"/>
-        <v>61.130672926447573</v>
+        <v>66.505280519273242</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
@@ -12723,20 +12735,20 @@
         <v>256</v>
       </c>
       <c r="C122">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="D122">
-        <v>85486</v>
+        <v>83851</v>
       </c>
       <c r="E122">
-        <v>126450</v>
+        <v>124747</v>
       </c>
       <c r="F122">
         <v>2499</v>
       </c>
       <c r="G122" s="2">
         <f t="shared" si="3"/>
-        <v>61.029196367542234</v>
+        <v>61.130672926447573</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -12747,20 +12759,20 @@
         <v>256</v>
       </c>
       <c r="C123">
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="D123">
-        <v>85629</v>
+        <v>85486</v>
       </c>
       <c r="E123">
-        <v>126679</v>
+        <v>126450</v>
       </c>
       <c r="F123">
         <v>2499</v>
       </c>
       <c r="G123" s="2">
         <f t="shared" si="3"/>
-        <v>60.90133982947625</v>
+        <v>61.029196367542234</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
@@ -12771,20 +12783,20 @@
         <v>256</v>
       </c>
       <c r="C124">
-        <v>256</v>
+        <v>512</v>
       </c>
       <c r="D124">
-        <v>86211</v>
+        <v>85629</v>
       </c>
       <c r="E124">
-        <v>127263</v>
+        <v>126679</v>
       </c>
       <c r="F124">
         <v>2499</v>
       </c>
       <c r="G124" s="2">
         <f t="shared" si="3"/>
-        <v>60.898372795478906</v>
+        <v>60.90133982947625</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -12795,20 +12807,20 @@
         <v>256</v>
       </c>
       <c r="C125">
-        <v>32</v>
+        <v>256</v>
       </c>
       <c r="D125">
-        <v>85860</v>
+        <v>86211</v>
       </c>
       <c r="E125">
-        <v>127512</v>
+        <v>127263</v>
       </c>
       <c r="F125">
         <v>2499</v>
       </c>
       <c r="G125" s="2">
         <f t="shared" si="3"/>
-        <v>60.021127436857775</v>
+        <v>60.898372795478906</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
@@ -12819,20 +12831,20 @@
         <v>256</v>
       </c>
       <c r="C126">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D126">
-        <v>89364</v>
+        <v>85860</v>
       </c>
       <c r="E126">
-        <v>134477</v>
+        <v>127512</v>
       </c>
       <c r="F126">
         <v>2499</v>
       </c>
       <c r="G126" s="2">
         <f t="shared" si="3"/>
-        <v>55.416398820739033</v>
+        <v>60.021127436857775</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
@@ -12843,23 +12855,50 @@
         <v>256</v>
       </c>
       <c r="C127">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D127">
-        <v>113816</v>
+        <v>89364</v>
       </c>
       <c r="E127">
-        <v>167035</v>
+        <v>134477</v>
       </c>
       <c r="F127">
         <v>2499</v>
       </c>
       <c r="G127" s="2">
         <f t="shared" si="3"/>
+        <v>55.416398820739033</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>8</v>
+      </c>
+      <c r="B128">
+        <v>256</v>
+      </c>
+      <c r="C128">
+        <v>8</v>
+      </c>
+      <c r="D128">
+        <v>113816</v>
+      </c>
+      <c r="E128">
+        <v>167035</v>
+      </c>
+      <c r="F128">
+        <v>2499</v>
+      </c>
+      <c r="G128" s="2">
+        <f t="shared" si="3"/>
         <v>46.975704165805446</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:I128">
+    <sortCondition descending="1" ref="G1:G128"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -19098,7 +19137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17DC667B-8D7F-45AA-BE88-D48E7C8ADA3A}">
   <dimension ref="A1:I127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>

</xml_diff>